<commit_message>
script export timetable to DB
</commit_message>
<xml_diff>
--- a/e_diary/timetable.xlsx
+++ b/e_diary/timetable.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="55">
   <si>
     <t>День</t>
   </si>
@@ -26,9 +26,6 @@
     <t>Предмет</t>
   </si>
   <si>
-    <t xml:space="preserve">ПН </t>
-  </si>
-  <si>
     <t>ВТ</t>
   </si>
   <si>
@@ -92,15 +89,9 @@
     <t>Учитель</t>
   </si>
   <si>
-    <t>Английския язык</t>
-  </si>
-  <si>
     <t>История</t>
   </si>
   <si>
-    <t>Хореогрфия</t>
-  </si>
-  <si>
     <t>Природоведение</t>
   </si>
   <si>
@@ -164,9 +155,6 @@
     <t>Татьяна Львовна Николаева</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Галина Александровна Маратова</t>
   </si>
   <si>
@@ -189,6 +177,9 @@
   </si>
   <si>
     <t>Николаева Надежда Константиновна</t>
+  </si>
+  <si>
+    <t>ПН</t>
   </si>
 </sst>
 </file>
@@ -222,12 +213,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -283,6 +268,14 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -569,90 +562,85 @@
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -962,10 +950,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -978,482 +966,475 @@
     <col min="8" max="8" width="36.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:4" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="28"/>
+    </row>
+    <row r="2" spans="1:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="34" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="15" t="s">
+      <c r="D3" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="30"/>
+      <c r="B4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="30"/>
+      <c r="B5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="30"/>
+      <c r="B6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="30"/>
+      <c r="B7" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="30"/>
+      <c r="B8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="11"/>
+      <c r="D8" s="8"/>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="31"/>
+      <c r="B9" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="12"/>
+      <c r="D9" s="10"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="10"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="11" t="s">
+      <c r="D10" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="30"/>
+      <c r="B11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C11" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="30"/>
+      <c r="B12" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="30"/>
+      <c r="B13" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="30"/>
+      <c r="B14" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="30"/>
+      <c r="B15" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="31"/>
+      <c r="B16" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="12"/>
+      <c r="D16" s="10"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="25" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="36"/>
-      <c r="B4" s="11" t="s">
+      <c r="D17" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="24"/>
+      <c r="B18" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="24"/>
+      <c r="B19" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C19" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="24"/>
+      <c r="B20" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="24"/>
+      <c r="B21" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="11"/>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="24"/>
+      <c r="B22" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="11"/>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:4" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="25"/>
+      <c r="B23" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="12"/>
+      <c r="D23" s="10"/>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="24"/>
+      <c r="B25" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="24"/>
+      <c r="B26" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="24"/>
+      <c r="B27" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D27" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="24"/>
+      <c r="B28" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="24"/>
+      <c r="B29" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="11"/>
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="25"/>
+      <c r="B30" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="12"/>
+      <c r="D30" s="10"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="24"/>
+      <c r="B32" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="24"/>
+      <c r="B33" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" s="22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="24"/>
+      <c r="B34" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="24"/>
+      <c r="B35" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="36"/>
-      <c r="B5" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="36"/>
-      <c r="B6" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="28" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="36"/>
-      <c r="B7" s="11" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="24"/>
+      <c r="B36" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="36"/>
-      <c r="B8" s="11" t="s">
+      <c r="C36" s="11"/>
+      <c r="D36" s="3"/>
+    </row>
+    <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="25"/>
+      <c r="B37" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="9"/>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="37"/>
-      <c r="B9" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="13"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="36"/>
-      <c r="B11" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="25" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="36"/>
-      <c r="B12" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="27" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="36"/>
-      <c r="B13" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="36"/>
-      <c r="B14" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="36"/>
-      <c r="B15" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="37"/>
-      <c r="B16" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="17"/>
-      <c r="D16" s="13"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
-      <c r="B18" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
-      <c r="B19" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="27" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="30"/>
-      <c r="B20" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="30"/>
-      <c r="B21" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="5"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="30"/>
-      <c r="B22" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="4"/>
-    </row>
-    <row r="23" spans="1:5" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="31"/>
-      <c r="B23" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" s="17"/>
-      <c r="D23" s="13"/>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="30"/>
-      <c r="B25" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E25" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="30"/>
-      <c r="B26" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="D26" s="27" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="30"/>
-      <c r="B27" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="30"/>
-      <c r="B28" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="30"/>
-      <c r="B29" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C29" s="14"/>
-      <c r="D29" s="4"/>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="31"/>
-      <c r="B30" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="C30" s="17"/>
-      <c r="D30" s="13"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C31" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="30"/>
-      <c r="B32" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C32" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="30"/>
-      <c r="B33" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C33" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D33" s="27" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="30"/>
-      <c r="B34" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C34" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="30"/>
-      <c r="B35" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C35" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="30"/>
-      <c r="B36" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C36" s="14"/>
-      <c r="D36" s="4"/>
-    </row>
-    <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="31"/>
-      <c r="B37" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="C37" s="17"/>
-      <c r="D37" s="13"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="10"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B38" s="11" t="s">
+      <c r="C38" s="11"/>
+      <c r="D38" s="5"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="24"/>
+      <c r="B39" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C38" s="14"/>
-      <c r="D38" s="6"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="30"/>
-      <c r="B39" s="11" t="s">
+      <c r="C39" s="11"/>
+      <c r="D39" s="7"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="24"/>
+      <c r="B40" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C39" s="14"/>
-      <c r="D39" s="8"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="30"/>
-      <c r="B40" s="11" t="s">
+      <c r="C40" s="11"/>
+      <c r="D40" s="6"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="24"/>
+      <c r="B41" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C40" s="14"/>
-      <c r="D40" s="7"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="30"/>
-      <c r="B41" s="11" t="s">
+      <c r="C41" s="11"/>
+      <c r="D41" s="2"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="24"/>
+      <c r="B42" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C41" s="14"/>
-      <c r="D41" s="3"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="30"/>
-      <c r="B42" s="11" t="s">
+      <c r="C42" s="11"/>
+      <c r="D42" s="4"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="24"/>
+      <c r="B43" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C42" s="14"/>
-      <c r="D42" s="5"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="30"/>
-      <c r="B43" s="11" t="s">
+      <c r="C43" s="11"/>
+      <c r="D43" s="3"/>
+    </row>
+    <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="25"/>
+      <c r="B44" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C43" s="14"/>
-      <c r="D43" s="4"/>
-    </row>
-    <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="31"/>
-      <c r="B44" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="C44" s="17"/>
-      <c r="D44" s="13"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1485,166 +1466,166 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="26" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="17" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="22" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="B11" s="17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="22" t="s">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="22" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="22" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="22" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="22" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="22" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="23" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="21" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="21" t="s">
-        <v>54</v>
+      <c r="A22" s="16" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="21" t="s">
-        <v>56</v>
+      <c r="A24" s="16" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add new API for schedule, debug load_timetable, add new interfaces for main and timetable pages, add modal form
</commit_message>
<xml_diff>
--- a/e_diary/timetable.xlsx
+++ b/e_diary/timetable.xlsx
@@ -609,6 +609,18 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -624,23 +636,11 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -952,8 +952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -967,29 +967,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="28"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="32"/>
     </row>
     <row r="2" spans="1:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="26" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="27" t="s">
         <v>54</v>
       </c>
       <c r="B3" s="9" t="s">
@@ -1003,7 +1003,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
+      <c r="A4" s="33"/>
       <c r="B4" s="9" t="s">
         <v>9</v>
       </c>
@@ -1015,19 +1015,19 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="30"/>
+      <c r="A5" s="33"/>
       <c r="B5" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
+      <c r="A6" s="33"/>
       <c r="B6" s="9" t="s">
         <v>11</v>
       </c>
@@ -1039,7 +1039,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
+      <c r="A7" s="33"/>
       <c r="B7" s="9" t="s">
         <v>12</v>
       </c>
@@ -1051,7 +1051,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
+      <c r="A8" s="33"/>
       <c r="B8" s="9" t="s">
         <v>13</v>
       </c>
@@ -1059,7 +1059,7 @@
       <c r="D8" s="8"/>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="31"/>
+      <c r="A9" s="34"/>
       <c r="B9" s="13" t="s">
         <v>14</v>
       </c>
@@ -1067,7 +1067,7 @@
       <c r="D9" s="10"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="27" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="9" t="s">
@@ -1081,7 +1081,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
+      <c r="A11" s="33"/>
       <c r="B11" s="9" t="s">
         <v>9</v>
       </c>
@@ -1093,7 +1093,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="30"/>
+      <c r="A12" s="33"/>
       <c r="B12" s="9" t="s">
         <v>10</v>
       </c>
@@ -1105,7 +1105,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="30"/>
+      <c r="A13" s="33"/>
       <c r="B13" s="9" t="s">
         <v>11</v>
       </c>
@@ -1117,7 +1117,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
+      <c r="A14" s="33"/>
       <c r="B14" s="9" t="s">
         <v>12</v>
       </c>
@@ -1129,7 +1129,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="30"/>
+      <c r="A15" s="33"/>
       <c r="B15" s="9" t="s">
         <v>13</v>
       </c>
@@ -1141,7 +1141,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="31"/>
+      <c r="A16" s="34"/>
       <c r="B16" s="13" t="s">
         <v>14</v>
       </c>
@@ -1149,7 +1149,7 @@
       <c r="D16" s="10"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="29" t="s">
+      <c r="A17" s="27" t="s">
         <v>4</v>
       </c>
       <c r="B17" s="9" t="s">
@@ -1163,7 +1163,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="24"/>
+      <c r="A18" s="28"/>
       <c r="B18" s="9" t="s">
         <v>9</v>
       </c>
@@ -1175,7 +1175,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="24"/>
+      <c r="A19" s="28"/>
       <c r="B19" s="9" t="s">
         <v>10</v>
       </c>
@@ -1187,7 +1187,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="24"/>
+      <c r="A20" s="28"/>
       <c r="B20" s="9" t="s">
         <v>11</v>
       </c>
@@ -1199,7 +1199,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="24"/>
+      <c r="A21" s="28"/>
       <c r="B21" s="9" t="s">
         <v>12</v>
       </c>
@@ -1207,7 +1207,7 @@
       <c r="D21" s="4"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="24"/>
+      <c r="A22" s="28"/>
       <c r="B22" s="9" t="s">
         <v>13</v>
       </c>
@@ -1215,7 +1215,7 @@
       <c r="D22" s="3"/>
     </row>
     <row r="23" spans="1:4" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="25"/>
+      <c r="A23" s="29"/>
       <c r="B23" s="13" t="s">
         <v>14</v>
       </c>
@@ -1223,7 +1223,7 @@
       <c r="D23" s="10"/>
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="29" t="s">
+      <c r="A24" s="27" t="s">
         <v>5</v>
       </c>
       <c r="B24" s="9" t="s">
@@ -1237,7 +1237,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="24"/>
+      <c r="A25" s="28"/>
       <c r="B25" s="9" t="s">
         <v>9</v>
       </c>
@@ -1249,7 +1249,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="24"/>
+      <c r="A26" s="28"/>
       <c r="B26" s="9" t="s">
         <v>10</v>
       </c>
@@ -1261,7 +1261,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="24"/>
+      <c r="A27" s="28"/>
       <c r="B27" s="9" t="s">
         <v>11</v>
       </c>
@@ -1273,7 +1273,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="24"/>
+      <c r="A28" s="28"/>
       <c r="B28" s="9" t="s">
         <v>12</v>
       </c>
@@ -1285,7 +1285,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="24"/>
+      <c r="A29" s="28"/>
       <c r="B29" s="9" t="s">
         <v>13</v>
       </c>
@@ -1293,7 +1293,7 @@
       <c r="D29" s="3"/>
     </row>
     <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="25"/>
+      <c r="A30" s="29"/>
       <c r="B30" s="13" t="s">
         <v>14</v>
       </c>
@@ -1301,13 +1301,13 @@
       <c r="D30" s="10"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="29" t="s">
+      <c r="A31" s="27" t="s">
         <v>6</v>
       </c>
       <c r="B31" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D31" s="5" t="s">
@@ -1315,7 +1315,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="24"/>
+      <c r="A32" s="28"/>
       <c r="B32" s="9" t="s">
         <v>9</v>
       </c>
@@ -1327,7 +1327,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="24"/>
+      <c r="A33" s="28"/>
       <c r="B33" s="9" t="s">
         <v>10</v>
       </c>
@@ -1339,7 +1339,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="24"/>
+      <c r="A34" s="28"/>
       <c r="B34" s="9" t="s">
         <v>11</v>
       </c>
@@ -1351,7 +1351,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="24"/>
+      <c r="A35" s="28"/>
       <c r="B35" s="9" t="s">
         <v>12</v>
       </c>
@@ -1363,7 +1363,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="24"/>
+      <c r="A36" s="28"/>
       <c r="B36" s="9" t="s">
         <v>13</v>
       </c>
@@ -1371,7 +1371,7 @@
       <c r="D36" s="3"/>
     </row>
     <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="25"/>
+      <c r="A37" s="29"/>
       <c r="B37" s="13" t="s">
         <v>14</v>
       </c>
@@ -1379,7 +1379,7 @@
       <c r="D37" s="10"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="29" t="s">
+      <c r="A38" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B38" s="9" t="s">
@@ -1389,7 +1389,7 @@
       <c r="D38" s="5"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="24"/>
+      <c r="A39" s="28"/>
       <c r="B39" s="9" t="s">
         <v>9</v>
       </c>
@@ -1397,7 +1397,7 @@
       <c r="D39" s="7"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="24"/>
+      <c r="A40" s="28"/>
       <c r="B40" s="9" t="s">
         <v>10</v>
       </c>
@@ -1405,7 +1405,7 @@
       <c r="D40" s="6"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="24"/>
+      <c r="A41" s="28"/>
       <c r="B41" s="9" t="s">
         <v>11</v>
       </c>
@@ -1413,7 +1413,7 @@
       <c r="D41" s="2"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="24"/>
+      <c r="A42" s="28"/>
       <c r="B42" s="9" t="s">
         <v>12</v>
       </c>
@@ -1421,7 +1421,7 @@
       <c r="D42" s="4"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="24"/>
+      <c r="A43" s="28"/>
       <c r="B43" s="9" t="s">
         <v>13</v>
       </c>
@@ -1429,7 +1429,7 @@
       <c r="D43" s="3"/>
     </row>
     <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="25"/>
+      <c r="A44" s="29"/>
       <c r="B44" s="13" t="s">
         <v>14</v>
       </c>

</xml_diff>